<commit_message>
adicionando tempos individuais os algoritmos
</commit_message>
<xml_diff>
--- a/GraficoAlgoritmos.xlsx
+++ b/GraficoAlgoritmos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
   <si>
     <t xml:space="preserve">3 cidades</t>
   </si>
@@ -210,7 +210,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF6D6D"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
@@ -698,11 +698,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="74554417"/>
-        <c:axId val="62323524"/>
+        <c:axId val="39380092"/>
+        <c:axId val="62657167"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74554417"/>
+        <c:axId val="39380092"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,14 +734,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62323524"/>
+        <c:crossAx val="62657167"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62323524"/>
+        <c:axId val="62657167"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,7 +780,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74554417"/>
+        <c:crossAx val="39380092"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1181,11 +1181,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="66437706"/>
-        <c:axId val="98768346"/>
+        <c:axId val="83626783"/>
+        <c:axId val="93193412"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66437706"/>
+        <c:axId val="83626783"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,14 +1217,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98768346"/>
+        <c:crossAx val="93193412"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98768346"/>
+        <c:axId val="93193412"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1263,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66437706"/>
+        <c:crossAx val="83626783"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1565,11 +1565,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="56259643"/>
-        <c:axId val="60416499"/>
+        <c:axId val="20635905"/>
+        <c:axId val="69431037"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56259643"/>
+        <c:axId val="20635905"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,14 +1601,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60416499"/>
+        <c:crossAx val="69431037"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60416499"/>
+        <c:axId val="69431037"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1647,7 +1647,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56259643"/>
+        <c:crossAx val="20635905"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1793,11 +1793,14 @@
               <a:srgbClr val="004586"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="ff6d6d"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1810,7 +1813,7 @@
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -1867,12 +1870,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="27696943"/>
-        <c:axId val="11065638"/>
-        <c:axId val="61869620"/>
+        <c:axId val="11804278"/>
+        <c:axId val="50871321"/>
+        <c:axId val="99859197"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="27696943"/>
+        <c:axId val="11804278"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1900,14 +1903,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11065638"/>
+        <c:crossAx val="50871321"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11065638"/>
+        <c:axId val="50871321"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,7 +1953,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1972,11 +1975,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27696943"/>
+        <c:crossAx val="11804278"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="61869620"/>
+        <c:axId val="99859197"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2004,15 +2007,52 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11065638"/>
+        <c:crossAx val="50871321"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>TSP - Branch and Bound</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2020,18 +2060,749 @@
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="11"/>
+      <c:rotY val="25"/>
+      <c:rAngAx val="1"/>
+      <c:perspective val="40"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="cccccc"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$O$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Branch and Bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$P$30:$T$30</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15 Cidades</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$P$31:$T$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0156</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.957867</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86.773467</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4617.2788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:shape val="box"/>
+        <c:axId val="76718994"/>
+        <c:axId val="32857785"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="76718994"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="32857785"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="32857785"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76718994"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>TSP - Dynamic Programming</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="11"/>
+      <c:rotY val="25"/>
+      <c:rAngAx val="1"/>
+      <c:perspective val="40"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="cccccc"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$O$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dynamic Programming</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$P$54:$T$54</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15 Cidades</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$P$55:$T$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0272</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.290133</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.915867</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.436733</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:shape val="box"/>
+        <c:axId val="22364501"/>
+        <c:axId val="43873563"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="22364501"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="43873563"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43873563"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22364501"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="pt-BR" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>TSP - Genetic Algorithm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="11"/>
+      <c:rotY val="25"/>
+      <c:rAngAx val="1"/>
+      <c:perspective val="40"/>
+    </c:view3D>
+    <c:floor>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="cccccc"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$F$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Genetic Algorithm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$G$60:$K$60</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12 Cidades</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15 Cidades</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$G$61:$K$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.008267</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.108733</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5782</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.833867</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.592</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:shape val="box"/>
+        <c:axId val="749289"/>
+        <c:axId val="54468638"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="749289"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="54468638"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="54468638"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="pt-BR" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="749289"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
@@ -2051,7 +2822,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
+      <xdr:colOff>229320</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2059,7 +2830,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>342720</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2067,8 +2838,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5820480" y="0"/>
-        <a:ext cx="5756400" cy="3447360"/>
+        <a:off x="5820840" y="0"/>
+        <a:ext cx="5756040" cy="3447000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2081,15 +2852,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>228960</xdr:colOff>
+      <xdr:colOff>229320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>266400</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2097,8 +2868,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5820480" y="3528360"/>
-        <a:ext cx="5680080" cy="3437640"/>
+        <a:off x="5820840" y="3528720"/>
+        <a:ext cx="5679720" cy="3437280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2111,15 +2882,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>219600</xdr:colOff>
+      <xdr:colOff>219960</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>171720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>257040</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2127,8 +2898,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5811120" y="7204680"/>
-        <a:ext cx="5680080" cy="3437640"/>
+        <a:off x="5811480" y="7174440"/>
+        <a:ext cx="5679720" cy="3437280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2141,15 +2912,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>230400</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:colOff>255600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>52920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>200880</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:colOff>225720</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2157,12 +2928,102 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12290760" y="1632960"/>
-        <a:ext cx="5756040" cy="3242160"/>
+        <a:off x="12315960" y="1752120"/>
+        <a:ext cx="5755680" cy="3241800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>344880</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>100080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>324000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>103680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="12405240" y="6150240"/>
+        <a:ext cx="5764680" cy="3242160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>726840</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>123840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>481320</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>158040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="11961000" y="10715400"/>
+        <a:ext cx="5764320" cy="3242160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>565920</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>48600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>687600</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>39960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4505400" y="11943360"/>
+        <a:ext cx="5764320" cy="3229920"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2176,10 +3037,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:T41"/>
+  <dimension ref="A2:T61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5:T6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W69" activeCellId="0" sqref="W69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2414,6 +3275,43 @@
         <v>5.592</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P30" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q30" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="R30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="S30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T30" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P31" s="1" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="Q31" s="1" t="n">
+        <v>0.0156</v>
+      </c>
+      <c r="R31" s="1" t="n">
+        <v>0.957867</v>
+      </c>
+      <c r="S31" s="2" t="n">
+        <v>86.773467</v>
+      </c>
+      <c r="T31" s="2" t="n">
+        <v>4617.2788</v>
+      </c>
+    </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
@@ -2469,6 +3367,80 @@
         <v>1.833867</v>
       </c>
       <c r="F41" s="2" t="n">
+        <v>5.592</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P54" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q54" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="R54" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="S54" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T54" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P55" s="1" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="Q55" s="1" t="n">
+        <v>0.0272</v>
+      </c>
+      <c r="R55" s="1" t="n">
+        <v>0.290133</v>
+      </c>
+      <c r="S55" s="2" t="n">
+        <v>2.915867</v>
+      </c>
+      <c r="T55" s="2" t="n">
+        <v>37.436733</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G60" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="1" t="n">
+        <v>0.008267</v>
+      </c>
+      <c r="H61" s="1" t="n">
+        <v>0.108733</v>
+      </c>
+      <c r="I61" s="1" t="n">
+        <v>0.5782</v>
+      </c>
+      <c r="J61" s="2" t="n">
+        <v>1.833867</v>
+      </c>
+      <c r="K61" s="2" t="n">
         <v>5.592</v>
       </c>
     </row>

</xml_diff>